<commit_message>
update method and code overview power bi
</commit_message>
<xml_diff>
--- a/qualitative_analysis/analysis_interviews/discussion_interviews.xlsx
+++ b/qualitative_analysis/analysis_interviews/discussion_interviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSIA\Masterarbeit\masterarbeit\qualitative_analysis\analysis_interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFF1F1D9-5AD7-4D89-B10A-0D5986CE8B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB7AC6-9F46-4A19-9879-0793FF075B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AAD4A880-87EC-42E5-85B1-EE7FDF33FE9F}"/>
   </bookViews>
@@ -40,18 +40,18 @@
     <author>tc={3B5D74C2-44F6-42E8-AFE1-1622D6ED3961}</author>
     <author>tc={16AF918A-E63A-41E4-AF5C-C27919C059C0}</author>
     <author>tc={E7126033-1277-4C05-9F86-7F2A8A4D94CB}</author>
+    <author>tc={DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}</author>
     <author>tc={28214FA8-6A58-442E-8427-9177EC992467}</author>
     <author>tc={91259C45-B46E-4D53-BC57-8C22FC6033AB}</author>
-    <author>tc={DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}</author>
     <author>tc={AA6DBC2D-A8D6-463C-959C-265C90932472}</author>
     <author>tc={FBE8EEC7-0069-470D-984C-4C2F82714600}</author>
     <author>tc={D8849280-6633-4D49-BDEA-A250A3539327}</author>
     <author>tc={21559D19-BF82-4C86-AA2B-7E231FB4FEB7}</author>
     <author>tc={128186CA-9630-4CC8-A708-9BECBE75886A}</author>
-    <author>tc={081B9B85-C3B6-45A8-813E-E87CD82D2D2B}</author>
     <author>tc={E41A9744-FB15-400A-A665-1B4347DBD689}</author>
     <author>tc={E1523C86-F975-4CDD-A663-75001F9682C0}</author>
     <author>tc={306BE626-28BC-40FD-A56F-D146EC02F763}</author>
+    <author>tc={081B9B85-C3B6-45A8-813E-E87CD82D2D2B}</author>
     <author>tc={A69F88E7-A06D-4E90-A23B-F33E08B68C72}</author>
     <author>tc={D4BE409B-ABE2-4B52-B4C8-4DF4D33C84B1}</author>
     <author>tc={7965B565-C3D7-4E49-8EA0-BA9E20FC0518}</author>
@@ -59,11 +59,11 @@
     <author>tc={2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}</author>
     <author>tc={DA6C7196-A8C1-4C7D-AD3B-DF879B5ED94D}</author>
     <author>tc={60170D08-EA95-41EE-AF42-BD51A980D095}</author>
+    <author>tc={3933A3D9-C023-4C0E-BAD4-200816DDFDEC}</author>
     <author>tc={6F70D089-3A35-46EE-B091-FEBFB5972460}</author>
-    <author>tc={3933A3D9-C023-4C0E-BAD4-200816DDFDEC}</author>
   </authors>
   <commentList>
-    <comment ref="L5" authorId="0" shapeId="0" xr:uid="{F0C40FB9-0050-4F94-A1B4-D179CA8CF1B7}">
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{F0C40FB9-0050-4F94-A1B4-D179CA8CF1B7}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -71,7 +71,7 @@
     inkl. zu viele Talente, die man nicht mehr los wird. Bsp Unternehmen</t>
       </text>
     </comment>
-    <comment ref="L6" authorId="1" shapeId="0" xr:uid="{3B5D74C2-44F6-42E8-AFE1-1622D6ED3961}">
+    <comment ref="H6" authorId="1" shapeId="0" xr:uid="{3B5D74C2-44F6-42E8-AFE1-1622D6ED3961}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -87,7 +87,7 @@
     stabile Versionen</t>
       </text>
     </comment>
-    <comment ref="H7" authorId="3" shapeId="0" xr:uid="{E7126033-1277-4C05-9F86-7F2A8A4D94CB}">
+    <comment ref="J7" authorId="3" shapeId="0" xr:uid="{E7126033-1277-4C05-9F86-7F2A8A4D94CB}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -97,7 +97,17 @@
     Reintegration in die Gesellschaft</t>
       </text>
     </comment>
-    <comment ref="H8" authorId="4" shapeId="0" xr:uid="{28214FA8-6A58-442E-8427-9177EC992467}">
+    <comment ref="H8" authorId="4" shapeId="0" xr:uid="{DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Werte in Fleisch und Blut übergegangen; Junge Personen einbinden
+Antwort:
+    transparente Kommunikation</t>
+      </text>
+    </comment>
+    <comment ref="J8" authorId="5" shapeId="0" xr:uid="{28214FA8-6A58-442E-8427-9177EC992467}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -105,7 +115,7 @@
     Beitrag zur Gesellschaft</t>
       </text>
     </comment>
-    <comment ref="J8" authorId="5" shapeId="0" xr:uid="{91259C45-B46E-4D53-BC57-8C22FC6033AB}">
+    <comment ref="L8" authorId="6" shapeId="0" xr:uid="{91259C45-B46E-4D53-BC57-8C22FC6033AB}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -113,16 +123,6 @@
     Software, Marketing, Verwaltungstätigkeiten, - geldgeber finden</t>
       </text>
     </comment>
-    <comment ref="L8" authorId="6" shapeId="0" xr:uid="{DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}">
-      <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Werte in Fleisch und Blut übergegangen; Junge Personen einbinden
-Antwort:
-    transparente Kommunikation</t>
-      </text>
-    </comment>
     <comment ref="F11" authorId="7" shapeId="0" xr:uid="{AA6DBC2D-A8D6-463C-959C-265C90932472}">
       <text>
         <t>[Kommentarthread]
@@ -131,7 +131,7 @@
     Social Media - Facebook Marktplatz</t>
       </text>
     </comment>
-    <comment ref="J11" authorId="8" shapeId="0" xr:uid="{FBE8EEC7-0069-470D-984C-4C2F82714600}">
+    <comment ref="L11" authorId="8" shapeId="0" xr:uid="{FBE8EEC7-0069-470D-984C-4C2F82714600}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -141,7 +141,7 @@
     Gleichwertigkeit der Tätigkeiten, E4 &amp; E6</t>
       </text>
     </comment>
-    <comment ref="J12" authorId="9" shapeId="0" xr:uid="{D8849280-6633-4D49-BDEA-A250A3539327}">
+    <comment ref="L12" authorId="9" shapeId="0" xr:uid="{D8849280-6633-4D49-BDEA-A250A3539327}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -165,7 +165,51 @@
     kein Interesse an Technologie dahinter</t>
       </text>
     </comment>
-    <comment ref="B22" authorId="12" shapeId="0" xr:uid="{081B9B85-C3B6-45A8-813E-E87CD82D2D2B}">
+    <comment ref="D22" authorId="12" shapeId="0" xr:uid="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Reduktion Arbeitszeiten, Teilen von Arbeitsplätzen
+Antwort:
+    Privatleben
+Antwort:
+    Mobiles Arbeiten
+Antwort:
+    Desk Sharing - 7
+Antwort:
+    Stundenjobs
+Antwort:
+    führen auf Distanz und Vertrauen
+Antwort:
+    resilienz</t>
+      </text>
+    </comment>
+    <comment ref="B24" authorId="13" shapeId="0" xr:uid="{E1523C86-F975-4CDD-A663-75001F9682C0}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Flexibilitierung und Zeitbanken</t>
+      </text>
+    </comment>
+    <comment ref="B25" authorId="14" shapeId="0" xr:uid="{306BE626-28BC-40FD-A56F-D146EC02F763}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Überwachung oder Lean Start Up? Digital oder analog? Hierarchien verwerfen und nicht nur anpreisen!
+Antwort:
+    Einbinden der Mitarbeiter, Empowerment
+Antwort:
+    Community im Unternehmen, Identifikation mit dem Unternehmen
+Antwort:
+    scheitern - Unternehmertum ausprobieren
+Antwort:
+    Vorteil in Bewerbungen: soziale Kompetenzen zeigen und Nachweis dafür erbringen</t>
+      </text>
+    </comment>
+    <comment ref="D25" authorId="15" shapeId="0" xr:uid="{081B9B85-C3B6-45A8-813E-E87CD82D2D2B}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -175,50 +219,6 @@
     Agilität</t>
       </text>
     </comment>
-    <comment ref="H22" authorId="13" shapeId="0" xr:uid="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-      <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Reduktion Arbeitszeiten, Teilen von Arbeitsplätzen
-Antwort:
-    Privatleben
-Antwort:
-    Mobiles Arbeiten
-Antwort:
-    Desk Sharing - 7
-Antwort:
-    Stundenjobs
-Antwort:
-    führen auf Distanz und Vertrauen
-Antwort:
-    resilienz</t>
-      </text>
-    </comment>
-    <comment ref="F24" authorId="14" shapeId="0" xr:uid="{E1523C86-F975-4CDD-A663-75001F9682C0}">
-      <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Flexibilitierung und Zeitbanken</t>
-      </text>
-    </comment>
-    <comment ref="F25" authorId="15" shapeId="0" xr:uid="{306BE626-28BC-40FD-A56F-D146EC02F763}">
-      <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Überwachung oder Lean Start Up? Digital oder analog? Hierarchien verwerfen und nicht nur anpreisen!
-Antwort:
-    Einbinden der Mitarbeiter, Empowerment
-Antwort:
-    Community im Unternehmen, Identifikation mit dem Unternehmen
-Antwort:
-    scheitern - Unternehmertum ausprobieren
-Antwort:
-    Vorteil in Bewerbungen: soziale Kompetenzen zeigen und Nachweis dafür erbringen</t>
-      </text>
-    </comment>
     <comment ref="D28" authorId="16" shapeId="0" xr:uid="{A69F88E7-A06D-4E90-A23B-F33E08B68C72}">
       <text>
         <t>[Kommentarthread]
@@ -245,7 +245,7 @@
     Genossenschaften</t>
       </text>
     </comment>
-    <comment ref="B34" authorId="19" shapeId="0" xr:uid="{C63373C8-C318-4E2F-A818-7AF4C80A7803}">
+    <comment ref="B32" authorId="19" shapeId="0" xr:uid="{C63373C8-C318-4E2F-A818-7AF4C80A7803}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -253,7 +253,7 @@
     systemisches Denken und Verknüpfen fördern</t>
       </text>
     </comment>
-    <comment ref="B35" authorId="20" shapeId="0" xr:uid="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
+    <comment ref="B33" authorId="20" shapeId="0" xr:uid="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -269,7 +269,7 @@
     E6: Mehr leistung soll auch belohnt werden</t>
       </text>
     </comment>
-    <comment ref="F42" authorId="21" shapeId="0" xr:uid="{DA6C7196-A8C1-4C7D-AD3B-DF879B5ED94D}">
+    <comment ref="D35" authorId="21" shapeId="0" xr:uid="{DA6C7196-A8C1-4C7D-AD3B-DF879B5ED94D}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -277,7 +277,7 @@
     Corporate Digital Responsibility</t>
       </text>
     </comment>
-    <comment ref="B43" authorId="22" shapeId="0" xr:uid="{60170D08-EA95-41EE-AF42-BD51A980D095}">
+    <comment ref="D36" authorId="22" shapeId="0" xr:uid="{60170D08-EA95-41EE-AF42-BD51A980D095}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -293,7 +293,17 @@
     Prozesse automatisieren</t>
       </text>
     </comment>
-    <comment ref="B45" authorId="23" shapeId="0" xr:uid="{6F70D089-3A35-46EE-B091-FEBFB5972460}">
+    <comment ref="B38" authorId="23" shapeId="0" xr:uid="{3933A3D9-C023-4C0E-BAD4-200816DDFDEC}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    Unterpunkte: Datenschutz, Fehlendes Vertrauen, Diskriminierung
+Antwort:
+    Cyber Physische Systeme</t>
+      </text>
+    </comment>
+    <comment ref="D38" authorId="24" shapeId="0" xr:uid="{6F70D089-3A35-46EE-B091-FEBFB5972460}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -301,16 +311,6 @@
     Eigenverantwortung
 Antwort:
     kritisches Hinterfragen der Entscheidungen und der Technologie</t>
-      </text>
-    </comment>
-    <comment ref="D45" authorId="24" shapeId="0" xr:uid="{3933A3D9-C023-4C0E-BAD4-200816DDFDEC}">
-      <text>
-        <t>[Kommentarthread]
-Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
-Kommentar:
-    Unterpunkte: Datenschutz, Fehlendes Vertrauen, Diskriminierung
-Antwort:
-    Cyber Physische Systeme</t>
       </text>
     </comment>
   </commentList>
@@ -318,7 +318,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="165">
   <si>
     <t xml:space="preserve">Angebote </t>
   </si>
@@ -344,27 +344,15 @@
     <t xml:space="preserve">azyklisches Verhalten ausgleichen </t>
   </si>
   <si>
-    <t xml:space="preserve">Arbeitsmarkt </t>
-  </si>
-  <si>
     <t xml:space="preserve">Zukunftsprognosen </t>
   </si>
   <si>
-    <t xml:space="preserve">Beschäftigungsmodelle </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gesellschaft </t>
-  </si>
-  <si>
     <t xml:space="preserve">Bildung </t>
   </si>
   <si>
     <t xml:space="preserve">Technologisierung </t>
   </si>
   <si>
-    <t xml:space="preserve">Verständnis von Technik </t>
-  </si>
-  <si>
     <t xml:space="preserve">Transparentes Buchungssystem </t>
   </si>
   <si>
@@ -443,12 +431,6 @@
     <t>Analog/digital</t>
   </si>
   <si>
-    <t>weniger Betrug</t>
-  </si>
-  <si>
-    <t>E1, A49</t>
-  </si>
-  <si>
     <t>Entfremdung durch Digitalisierung</t>
   </si>
   <si>
@@ -489,12 +471,6 @@
   </si>
   <si>
     <t>E2, A2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Regionalität/Globalisierung </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nachfragezuwachs </t>
   </si>
   <si>
     <t xml:space="preserve">Technische Berufe </t>
@@ -655,10 +631,6 @@
   </si>
   <si>
     <t>E2, A25; E5, A16</t>
-  </si>
-  <si>
-    <t>E1, A20;
-E5, A18</t>
   </si>
   <si>
     <t>E4, A13; 
@@ -945,6 +917,16 @@
 E5, A14, A18; 
 E9, A46
 E10, A2, A12</t>
+  </si>
+  <si>
+    <t>Arbeitsmarkt/Gesellschaft/Bildung</t>
+  </si>
+  <si>
+    <t>Gesellschaft</t>
+  </si>
+  <si>
+    <t>E1, A20;
+E5, A18, A16</t>
   </si>
 </sst>
 </file>
@@ -960,10 +942,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Segoe UI"/>
-      <charset val="1"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -986,9 +970,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1311,43 +1299,43 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L5" dT="2021-06-09T09:55:10.48" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{F0C40FB9-0050-4F94-A1B4-D179CA8CF1B7}">
+  <threadedComment ref="H5" dT="2021-06-09T09:55:10.48" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{F0C40FB9-0050-4F94-A1B4-D179CA8CF1B7}">
     <text>inkl. zu viele Talente, die man nicht mehr los wird. Bsp Unternehmen</text>
   </threadedComment>
-  <threadedComment ref="L6" dT="2021-06-10T15:27:58.83" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{3B5D74C2-44F6-42E8-AFE1-1622D6ED3961}">
+  <threadedComment ref="H6" dT="2021-06-10T15:27:58.83" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{3B5D74C2-44F6-42E8-AFE1-1622D6ED3961}">
     <text>von anderen lernen</text>
   </threadedComment>
   <threadedComment ref="F7" dT="2021-06-09T20:55:17.72" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{16AF918A-E63A-41E4-AF5C-C27919C059C0}">
     <text>stabile Versionen</text>
   </threadedComment>
-  <threadedComment ref="H7" dT="2021-06-09T19:43:53.83" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E7126033-1277-4C05-9F86-7F2A8A4D94CB}">
+  <threadedComment ref="J7" dT="2021-06-09T19:43:53.83" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E7126033-1277-4C05-9F86-7F2A8A4D94CB}">
     <text>Freundschaften</text>
   </threadedComment>
-  <threadedComment ref="H7" dT="2021-06-09T19:52:05.30" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E57C1DE8-952D-4BF7-8EA9-7DA172F18D0C}" parentId="{E7126033-1277-4C05-9F86-7F2A8A4D94CB}">
+  <threadedComment ref="J7" dT="2021-06-09T19:52:05.30" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E57C1DE8-952D-4BF7-8EA9-7DA172F18D0C}" parentId="{E7126033-1277-4C05-9F86-7F2A8A4D94CB}">
     <text>Reintegration in die Gesellschaft</text>
   </threadedComment>
-  <threadedComment ref="H8" dT="2021-06-10T14:09:03.11" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{28214FA8-6A58-442E-8427-9177EC992467}">
+  <threadedComment ref="H8" dT="2021-06-09T21:07:13.09" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}">
+    <text>Werte in Fleisch und Blut übergegangen; Junge Personen einbinden</text>
+  </threadedComment>
+  <threadedComment ref="H8" dT="2021-06-10T14:52:27.11" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{2C4404B6-85F0-44EB-83F7-88D66F738FBE}" parentId="{DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}">
+    <text>transparente Kommunikation</text>
+  </threadedComment>
+  <threadedComment ref="J8" dT="2021-06-10T14:09:03.11" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{28214FA8-6A58-442E-8427-9177EC992467}">
     <text>Beitrag zur Gesellschaft</text>
   </threadedComment>
-  <threadedComment ref="J8" dT="2021-06-09T17:03:54.00" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{91259C45-B46E-4D53-BC57-8C22FC6033AB}">
+  <threadedComment ref="L8" dT="2021-06-09T17:03:54.00" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{91259C45-B46E-4D53-BC57-8C22FC6033AB}">
     <text>Software, Marketing, Verwaltungstätigkeiten, - geldgeber finden</text>
-  </threadedComment>
-  <threadedComment ref="L8" dT="2021-06-09T21:07:13.09" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}">
-    <text>Werte in Fleisch und Blut übergegangen; Junge Personen einbinden</text>
-  </threadedComment>
-  <threadedComment ref="L8" dT="2021-06-10T14:52:27.11" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{2C4404B6-85F0-44EB-83F7-88D66F738FBE}" parentId="{DB0BD1AE-2210-4A3F-9E98-9D0E5ECD0CA9}">
-    <text>transparente Kommunikation</text>
   </threadedComment>
   <threadedComment ref="F11" dT="2021-06-09T16:56:27.08" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{AA6DBC2D-A8D6-463C-959C-265C90932472}">
     <text>Social Media - Facebook Marktplatz</text>
   </threadedComment>
-  <threadedComment ref="J11" dT="2021-06-10T12:57:00.40" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{FBE8EEC7-0069-470D-984C-4C2F82714600}">
+  <threadedComment ref="L11" dT="2021-06-10T12:57:00.40" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{FBE8EEC7-0069-470D-984C-4C2F82714600}">
     <text>Auslöschung Berufsstände kritisch</text>
   </threadedComment>
-  <threadedComment ref="J11" dT="2021-06-10T12:57:10.22" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{BF803C8F-FB44-4CF4-9D12-DBB621CF4C25}" parentId="{FBE8EEC7-0069-470D-984C-4C2F82714600}">
+  <threadedComment ref="L11" dT="2021-06-10T12:57:10.22" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{BF803C8F-FB44-4CF4-9D12-DBB621CF4C25}" parentId="{FBE8EEC7-0069-470D-984C-4C2F82714600}">
     <text>Gleichwertigkeit der Tätigkeiten, E4 &amp; E6</text>
   </threadedComment>
-  <threadedComment ref="J12" dT="2021-06-09T18:30:39.35" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{D8849280-6633-4D49-BDEA-A250A3539327}">
+  <threadedComment ref="L12" dT="2021-06-09T18:30:39.35" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{D8849280-6633-4D49-BDEA-A250A3539327}">
     <text>warum kann ich die Leistung nicht einfach kaufen?</text>
   </threadedComment>
   <threadedComment ref="F13" dT="2021-06-09T16:57:47.08" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{21559D19-BF82-4C86-AA2B-7E231FB4FEB7}">
@@ -1356,50 +1344,50 @@
   <threadedComment ref="F14" dT="2021-06-09T19:27:39.89" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{128186CA-9630-4CC8-A708-9BECBE75886A}">
     <text>kein Interesse an Technologie dahinter</text>
   </threadedComment>
-  <threadedComment ref="B22" dT="2021-06-09T10:51:58.07" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{081B9B85-C3B6-45A8-813E-E87CD82D2D2B}">
+  <threadedComment ref="D22" dT="2021-06-09T10:38:47.91" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>Reduktion Arbeitszeiten, Teilen von Arbeitsplätzen</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2021-06-09T17:16:01.38" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{80208D3E-059C-4DBE-AD1A-4C312E5B9FA6}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>Privatleben</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2021-06-09T20:07:08.41" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{68C447DC-D635-420E-AB5D-645CEC24DFEC}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>Mobiles Arbeiten</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2021-06-09T20:09:32.02" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{46B73EC3-1CE3-4631-8EBB-A75E4DEA72A7}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>Desk Sharing - 7</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2021-06-10T15:28:11.01" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{813E7B04-00E1-411F-95AD-DFC232BB8A98}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>Stundenjobs</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2021-06-10T15:49:24.17" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{A3570E3D-DBC6-4DCB-88D9-6B427167852C}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>führen auf Distanz und Vertrauen</text>
+  </threadedComment>
+  <threadedComment ref="D22" dT="2021-06-10T15:54:20.12" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{0DECA075-C552-47D7-9942-F5C504B7A2BF}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
+    <text>resilienz</text>
+  </threadedComment>
+  <threadedComment ref="B24" dT="2021-06-09T20:36:00.36" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E1523C86-F975-4CDD-A663-75001F9682C0}">
+    <text>Flexibilitierung und Zeitbanken</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2021-06-09T20:09:15.87" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{306BE626-28BC-40FD-A56F-D146EC02F763}">
+    <text>Überwachung oder Lean Start Up? Digital oder analog? Hierarchien verwerfen und nicht nur anpreisen!</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2021-06-09T20:19:31.32" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{1D68940F-197A-4915-9EAD-7C5BD968A620}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
+    <text>Einbinden der Mitarbeiter, Empowerment</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2021-06-10T14:57:15.22" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{C480782E-1F32-480E-BE1A-FE8959911985}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
+    <text>Community im Unternehmen, Identifikation mit dem Unternehmen</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2021-06-10T15:31:30.42" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{964262C5-3721-45F4-A948-14BF0773169F}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
+    <text>scheitern - Unternehmertum ausprobieren</text>
+  </threadedComment>
+  <threadedComment ref="B25" dT="2021-06-10T15:36:00.52" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{7D88F0E5-786A-46F9-BDC6-909886B73B45}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
+    <text>Vorteil in Bewerbungen: soziale Kompetenzen zeigen und Nachweis dafür erbringen</text>
+  </threadedComment>
+  <threadedComment ref="D25" dT="2021-06-09T10:51:58.07" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{081B9B85-C3B6-45A8-813E-E87CD82D2D2B}">
     <text>Verbindung mit Sharing Economy, Beispiel Autobauer</text>
   </threadedComment>
-  <threadedComment ref="B22" dT="2021-06-09T17:24:40.28" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{7460AD35-96EB-426F-AAB1-55205C194460}" parentId="{081B9B85-C3B6-45A8-813E-E87CD82D2D2B}">
+  <threadedComment ref="D25" dT="2021-06-09T17:24:40.28" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{7460AD35-96EB-426F-AAB1-55205C194460}" parentId="{081B9B85-C3B6-45A8-813E-E87CD82D2D2B}">
     <text>Agilität</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-09T10:38:47.91" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>Reduktion Arbeitszeiten, Teilen von Arbeitsplätzen</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-09T17:16:01.38" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{80208D3E-059C-4DBE-AD1A-4C312E5B9FA6}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>Privatleben</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-09T20:07:08.41" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{68C447DC-D635-420E-AB5D-645CEC24DFEC}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>Mobiles Arbeiten</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-09T20:09:32.02" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{46B73EC3-1CE3-4631-8EBB-A75E4DEA72A7}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>Desk Sharing - 7</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-10T15:28:11.01" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{813E7B04-00E1-411F-95AD-DFC232BB8A98}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>Stundenjobs</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-10T15:49:24.17" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{A3570E3D-DBC6-4DCB-88D9-6B427167852C}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>führen auf Distanz und Vertrauen</text>
-  </threadedComment>
-  <threadedComment ref="H22" dT="2021-06-10T15:54:20.12" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{0DECA075-C552-47D7-9942-F5C504B7A2BF}" parentId="{E41A9744-FB15-400A-A665-1B4347DBD689}">
-    <text>resilienz</text>
-  </threadedComment>
-  <threadedComment ref="F24" dT="2021-06-09T20:36:00.36" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{E1523C86-F975-4CDD-A663-75001F9682C0}">
-    <text>Flexibilitierung und Zeitbanken</text>
-  </threadedComment>
-  <threadedComment ref="F25" dT="2021-06-09T20:09:15.87" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{306BE626-28BC-40FD-A56F-D146EC02F763}">
-    <text>Überwachung oder Lean Start Up? Digital oder analog? Hierarchien verwerfen und nicht nur anpreisen!</text>
-  </threadedComment>
-  <threadedComment ref="F25" dT="2021-06-09T20:19:31.32" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{1D68940F-197A-4915-9EAD-7C5BD968A620}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
-    <text>Einbinden der Mitarbeiter, Empowerment</text>
-  </threadedComment>
-  <threadedComment ref="F25" dT="2021-06-10T14:57:15.22" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{C480782E-1F32-480E-BE1A-FE8959911985}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
-    <text>Community im Unternehmen, Identifikation mit dem Unternehmen</text>
-  </threadedComment>
-  <threadedComment ref="F25" dT="2021-06-10T15:31:30.42" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{964262C5-3721-45F4-A948-14BF0773169F}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
-    <text>scheitern - Unternehmertum ausprobieren</text>
-  </threadedComment>
-  <threadedComment ref="F25" dT="2021-06-10T15:36:00.52" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{7D88F0E5-786A-46F9-BDC6-909886B73B45}" parentId="{306BE626-28BC-40FD-A56F-D146EC02F763}">
-    <text>Vorteil in Bewerbungen: soziale Kompetenzen zeigen und Nachweis dafür erbringen</text>
   </threadedComment>
   <threadedComment ref="D28" dT="2021-06-09T20:11:54.77" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{A69F88E7-A06D-4E90-A23B-F33E08B68C72}">
     <text>Büro als sozialer Ort</text>
@@ -1413,692 +1401,724 @@
   <threadedComment ref="D30" dT="2021-06-09T17:26:52.36" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{7965B565-C3D7-4E49-8EA0-BA9E20FC0518}">
     <text>Genossenschaften</text>
   </threadedComment>
-  <threadedComment ref="B34" dT="2021-06-09T17:22:20.89" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{C63373C8-C318-4E2F-A818-7AF4C80A7803}">
+  <threadedComment ref="B32" dT="2021-06-09T17:22:20.89" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{C63373C8-C318-4E2F-A818-7AF4C80A7803}">
     <text>systemisches Denken und Verknüpfen fördern</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2021-06-09T10:30:56.17" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
+  <threadedComment ref="B33" dT="2021-06-09T10:30:56.17" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
     <text>flexibler, spannender, online, Interaktionen</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2021-06-09T19:35:11.52" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{CA2C9D2C-D6A5-4DE5-981E-CA190CA21DF4}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
+  <threadedComment ref="B33" dT="2021-06-09T19:35:11.52" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{CA2C9D2C-D6A5-4DE5-981E-CA190CA21DF4}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
     <text>Familie in der Verantwortung</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2021-06-09T20:24:59.46" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{F0F54C87-2BA7-4CE3-93C4-C1C6E04F8066}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
+  <threadedComment ref="B33" dT="2021-06-09T20:24:59.46" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{F0F54C87-2BA7-4CE3-93C4-C1C6E04F8066}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
     <text>kein Bulemielernen; Vorbereitung auf Flexibilität</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2021-06-09T20:25:17.64" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{D4E5B085-B398-4F5F-BB04-D3B14E08199D}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
+  <threadedComment ref="B33" dT="2021-06-09T20:25:17.64" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{D4E5B085-B398-4F5F-BB04-D3B14E08199D}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
     <text>Eigenverantwortun, selbstorganisiertes Lernen</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2021-06-10T13:25:06.60" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{278A20E5-9A20-402D-8E37-463C55F6E22A}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
+  <threadedComment ref="B33" dT="2021-06-10T13:25:06.60" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{278A20E5-9A20-402D-8E37-463C55F6E22A}" parentId="{2F1FBAF4-3E31-4D48-8914-3D49EA27F11C}">
     <text>E6: Mehr leistung soll auch belohnt werden</text>
   </threadedComment>
-  <threadedComment ref="F42" dT="2021-06-09T20:04:32.75" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{DA6C7196-A8C1-4C7D-AD3B-DF879B5ED94D}">
+  <threadedComment ref="D35" dT="2021-06-09T20:04:32.75" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{DA6C7196-A8C1-4C7D-AD3B-DF879B5ED94D}">
     <text>Corporate Digital Responsibility</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2021-06-09T10:23:29.21" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{60170D08-EA95-41EE-AF42-BD51A980D095}">
+  <threadedComment ref="D36" dT="2021-06-09T10:23:29.21" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{60170D08-EA95-41EE-AF42-BD51A980D095}">
     <text>am Arbeitsplatz, für Prozesse und für Menschen in der Interaktion oder Aufrechterhaltung der Lebensqualität</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2021-06-09T17:45:23.57" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{42A1DE6E-553C-4AE7-ACE8-06D257ECAAE1}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
+  <threadedComment ref="D36" dT="2021-06-09T17:45:23.57" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{42A1DE6E-553C-4AE7-ACE8-06D257ECAAE1}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
     <text>cyber physische systeme</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2021-06-09T20:13:10.03" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{310CC212-F6B6-4C63-8CE5-6F5B01B5CDB8}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
+  <threadedComment ref="D36" dT="2021-06-09T20:13:10.03" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{310CC212-F6B6-4C63-8CE5-6F5B01B5CDB8}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
     <text>mehr Freiraum</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2021-06-09T20:21:04.56" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{2BAAD563-A972-43EE-84B5-AEF041616C3C}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
+  <threadedComment ref="D36" dT="2021-06-09T20:21:04.56" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{2BAAD563-A972-43EE-84B5-AEF041616C3C}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
     <text>langweilige, repetitive, schwere köölrperliche Arbeiten, unwürdige Arbeiten</text>
   </threadedComment>
-  <threadedComment ref="B43" dT="2021-06-09T20:22:57.54" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{FDAEB167-A6C0-4BC8-85C7-7003439A9888}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
+  <threadedComment ref="D36" dT="2021-06-09T20:22:57.54" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{FDAEB167-A6C0-4BC8-85C7-7003439A9888}" parentId="{60170D08-EA95-41EE-AF42-BD51A980D095}">
     <text>Prozesse automatisieren</text>
   </threadedComment>
-  <threadedComment ref="B45" dT="2021-06-09T19:29:50.90" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{6F70D089-3A35-46EE-B091-FEBFB5972460}">
+  <threadedComment ref="B38" dT="2021-06-09T10:25:27.80" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{3933A3D9-C023-4C0E-BAD4-200816DDFDEC}">
+    <text>Unterpunkte: Datenschutz, Fehlendes Vertrauen, Diskriminierung</text>
+  </threadedComment>
+  <threadedComment ref="B38" dT="2021-06-09T17:47:09.99" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{8AFBCED2-5BE6-4BEC-BEA6-F17B35F82E48}" parentId="{3933A3D9-C023-4C0E-BAD4-200816DDFDEC}">
+    <text>Cyber Physische Systeme</text>
+  </threadedComment>
+  <threadedComment ref="D38" dT="2021-06-09T19:29:50.90" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{6F70D089-3A35-46EE-B091-FEBFB5972460}">
     <text>Eigenverantwortung</text>
   </threadedComment>
-  <threadedComment ref="B45" dT="2021-06-10T14:03:29.12" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{D4A65CCF-566F-46C5-903F-7F1DB93CAE7A}" parentId="{6F70D089-3A35-46EE-B091-FEBFB5972460}">
+  <threadedComment ref="D38" dT="2021-06-10T14:03:29.12" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{D4A65CCF-566F-46C5-903F-7F1DB93CAE7A}" parentId="{6F70D089-3A35-46EE-B091-FEBFB5972460}">
     <text>kritisches Hinterfragen der Entscheidungen und der Technologie</text>
-  </threadedComment>
-  <threadedComment ref="D45" dT="2021-06-09T10:25:27.80" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{3933A3D9-C023-4C0E-BAD4-200816DDFDEC}">
-    <text>Unterpunkte: Datenschutz, Fehlendes Vertrauen, Diskriminierung</text>
-  </threadedComment>
-  <threadedComment ref="D45" dT="2021-06-09T17:47:09.99" personId="{A2871FC7-3CB7-4F0A-B7E1-9BEF4281C986}" id="{8AFBCED2-5BE6-4BEC-BEA6-F17B35F82E48}" parentId="{3933A3D9-C023-4C0E-BAD4-200816DDFDEC}">
-    <text>Cyber Physische Systeme</text>
   </threadedComment>
 </ThreadedComments>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68711D56-1947-4B10-A47F-6F5FB0908BE9}">
-  <dimension ref="A1:M46"/>
+  <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C5" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="31.77734375" customWidth="1"/>
-    <col min="8" max="8" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.21875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.21875" customWidth="1"/>
-    <col min="12" max="12" width="28.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.21875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5546875" style="1"/>
+    <col min="8" max="8" width="34" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" customWidth="1"/>
+    <col min="14" max="14" width="28.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M4" s="2"/>
+    </row>
+    <row r="5" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="J5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3"/>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H6" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="J6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="L6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="M6" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H7" t="s">
+        <v>100</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="J7" t="s">
+        <v>69</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="F4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="M7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="H8" t="s">
+        <v>110</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="J8" t="s">
+        <v>94</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="L8" t="s">
+        <v>26</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="B9" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="H9" t="s">
+        <v>159</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J9" t="s">
+        <v>109</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="L9" t="s">
+        <v>67</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="3"/>
+      <c r="B10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="L10" t="s">
+        <v>79</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="L11" t="s">
+        <v>83</v>
+      </c>
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="L12" t="s">
+        <v>93</v>
+      </c>
+      <c r="M12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="L14" t="s">
+        <v>155</v>
+      </c>
+      <c r="M14" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="1" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+    </row>
+    <row r="20" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:11" ht="105" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A25" s="3"/>
+      <c r="B25" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="D27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D30" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D31" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="72" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D36" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="E5" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="1" t="s">
+      <c r="E36" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D37" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="H5" t="s">
-        <v>17</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="J5" t="s">
-        <v>29</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="L5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" t="s">
-        <v>109</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="L6" t="s">
-        <v>33</v>
-      </c>
-      <c r="M6" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" t="s">
-        <v>123</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="E37" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B39" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C39" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="F7" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" t="s">
-        <v>54</v>
-      </c>
-      <c r="H7" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" t="s">
-        <v>108</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="72" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>124</v>
-      </c>
-      <c r="E8" t="s">
-        <v>125</v>
-      </c>
-      <c r="F8" t="s">
-        <v>78</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="H8" t="s">
-        <v>102</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L8" t="s">
-        <v>119</v>
-      </c>
-      <c r="M8" s="1" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B9" t="s">
-        <v>76</v>
-      </c>
-      <c r="C9" t="s">
-        <v>74</v>
-      </c>
-      <c r="F9" t="s">
-        <v>80</v>
-      </c>
-      <c r="G9" t="s">
-        <v>79</v>
-      </c>
-      <c r="H9" t="s">
-        <v>118</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J9" t="s">
-        <v>75</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="L9" t="s">
-        <v>168</v>
-      </c>
-      <c r="M9" s="1" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="F10" t="s">
-        <v>81</v>
-      </c>
-      <c r="G10" t="s">
-        <v>82</v>
-      </c>
-      <c r="J10" t="s">
-        <v>87</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" t="s">
-        <v>117</v>
-      </c>
-      <c r="F11" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J11" t="s">
-        <v>91</v>
-      </c>
-      <c r="K11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" t="s">
-        <v>122</v>
-      </c>
-      <c r="F12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="J12" t="s">
-        <v>101</v>
-      </c>
-      <c r="K12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" t="s">
-        <v>145</v>
-      </c>
-      <c r="C13" t="s">
-        <v>146</v>
-      </c>
-      <c r="F13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
-        <v>147</v>
-      </c>
-      <c r="C14" t="s">
-        <v>146</v>
-      </c>
-      <c r="F14" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="J14" t="s">
-        <v>164</v>
-      </c>
-      <c r="K14" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B15" t="s">
-        <v>148</v>
-      </c>
-      <c r="C15" t="s">
-        <v>146</v>
-      </c>
-      <c r="F15" t="s">
-        <v>128</v>
-      </c>
-      <c r="G15" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
-      <c r="F20" t="s">
-        <v>4</v>
-      </c>
-      <c r="H20" t="s">
-        <v>9</v>
-      </c>
-      <c r="J20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B21" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" t="s">
-        <v>44</v>
-      </c>
-      <c r="D21" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="H21" t="s">
-        <v>61</v>
-      </c>
-      <c r="I21" t="s">
-        <v>60</v>
-      </c>
-      <c r="J21" t="s">
-        <v>45</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
-        <v>62</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="F22" t="s">
-        <v>36</v>
-      </c>
-      <c r="G22" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" t="s">
-        <v>66</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="F23" t="s">
-        <v>49</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="H23" t="s">
-        <v>92</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="F24" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="H24" t="s">
-        <v>93</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="72" x14ac:dyDescent="0.3">
-      <c r="F25" t="s">
-        <v>112</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>11</v>
-      </c>
-      <c r="B27" t="s">
-        <v>4</v>
-      </c>
-      <c r="D27" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B28" t="s">
-        <v>37</v>
-      </c>
-      <c r="C28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B29" t="s">
-        <v>40</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D30" t="s">
-        <v>71</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="D31" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>12</v>
-      </c>
-      <c r="B33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="D34" t="s">
-        <v>106</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>64</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-      <c r="B41" t="s">
-        <v>14</v>
-      </c>
-      <c r="D41" t="s">
-        <v>4</v>
-      </c>
-      <c r="F41" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="72" x14ac:dyDescent="0.3">
-      <c r="B42" t="s">
-        <v>41</v>
-      </c>
-      <c r="C42" t="s">
-        <v>42</v>
-      </c>
-      <c r="D42" t="s">
-        <v>46</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="F42" t="s">
-        <v>98</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D43" t="s">
-        <v>47</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B44" t="s">
-        <v>94</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D44" t="s">
-        <v>51</v>
-      </c>
-      <c r="E44" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B45" t="s">
-        <v>107</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D45" t="s">
-        <v>95</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="D46" t="s">
-        <v>65</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
upload infrastructure proposal draft
</commit_message>
<xml_diff>
--- a/qualitative_analysis/analysis_interviews/discussion_interviews.xlsx
+++ b/qualitative_analysis/analysis_interviews/discussion_interviews.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSIA\Masterarbeit\masterarbeit\qualitative_analysis\analysis_interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69FB7AC6-9F46-4A19-9879-0793FF075B43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52368B89-940D-476A-969F-0C387474F779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AAD4A880-87EC-42E5-85B1-EE7FDF33FE9F}"/>
   </bookViews>
@@ -1456,7 +1456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68711D56-1947-4B10-A47F-6F5FB0908BE9}">
   <dimension ref="A1:M39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -1928,7 +1928,7 @@
       </c>
       <c r="F24" s="3"/>
     </row>
-    <row r="25" spans="1:11" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="1" t="s">
         <v>103</v>

</xml_diff>